<commit_message>
Added table columns Added additional checks Added left margin
</commit_message>
<xml_diff>
--- a/TestRun/Mitarbeiter.xlsx
+++ b/TestRun/Mitarbeiter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\source\repos\CovidBulkBavaria\TestRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1F8C6C-F36F-4965-ADCD-7D1DC2024D1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3430E977-7D4D-49D6-83EE-76B6E23B38BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21924" windowHeight="13176" xr2:uid="{E6F5B6AA-BBA1-4225-99F1-6FBB0D36E666}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
   <si>
     <t>Vorname</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>Komissar</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Ersttestung</t>
+  </si>
+  <si>
+    <t>Symptome</t>
+  </si>
+  <si>
+    <t>Übermittelung an GSA</t>
   </si>
 </sst>
 </file>
@@ -538,18 +556,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC85D635-82D9-45C0-8408-F078E573257E}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -577,8 +599,20 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -589,7 +623,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>35777</v>
+        <v>33219</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -606,8 +640,20 @@
       <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -635,8 +681,20 @@
       <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -664,8 +722,20 @@
       <c r="I4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -693,8 +763,20 @@
       <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -722,8 +804,20 @@
       <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -751,8 +845,20 @@
       <c r="I7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -780,8 +886,20 @@
       <c r="I8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -809,8 +927,20 @@
       <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -838,8 +968,20 @@
       <c r="I10" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -867,8 +1009,20 @@
       <c r="I11" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -895,6 +1049,18 @@
       </c>
       <c r="I12" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>